<commit_message>
Created fitSlicesGauss.h and cmap.h
</commit_message>
<xml_diff>
--- a/makePlots/gain_vs_MIP_plots.xlsx
+++ b/makePlots/gain_vs_MIP_plots.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/samuelgrant/Documents/gm2/gain_corrections/makePlots/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{61DABBFC-92CB-D444-9D41-04F37B25E929}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C406D1D4-7B81-CD4C-8E08-542C6ABD45F3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="980" yWindow="1440" windowWidth="27240" windowHeight="15400" xr2:uid="{9E573E0F-DE19-EC4E-9BD7-BD69877D8C02}"/>
   </bookViews>
@@ -4787,7 +4787,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D0B2C54-F224-754D-9A6A-DE5E962ED340}">
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="H21" zoomScale="258" zoomScaleNormal="258" workbookViewId="0">
       <selection activeCell="S31" sqref="S31"/>
     </sheetView>
   </sheetViews>

</xml_diff>